<commit_message>
done reading ferre data, added class for storing ferre data
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IdeaProjects\FerreTriangle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\KtlnProjects\FerreTriangle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10788"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10785"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -68,12 +68,36 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -88,12 +112,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -377,16 +405,16 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -397,8 +425,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -408,8 +436,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -419,8 +447,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -430,8 +458,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">

</xml_diff>